<commit_message>
edit csv for dataset5
</commit_message>
<xml_diff>
--- a/APS360_Project_Dataset/dataset5/labels.xlsx
+++ b/APS360_Project_Dataset/dataset5/labels.xlsx
@@ -11,7 +11,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="161">
+  <si>
+    <t>image_num</t>
+  </si>
+  <si>
+    <t>card_num</t>
+  </si>
   <si>
     <t>1</t>
   </si>
@@ -521,9 +527,12 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
@@ -762,159 +771,159 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="s">
+      <c r="A15" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="s">
+      <c r="A17" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="1" t="s">
+      <c r="A19" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="1" t="s">
+      <c r="A20" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="1" t="s">
+      <c r="A21" s="2" t="s">
         <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -922,475 +931,483 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="1" t="s">
+      <c r="A22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="1" t="s">
+      <c r="A23" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="1" t="s">
+      <c r="A24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
+      <c r="A25" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="1" t="s">
+      <c r="A26" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="1" t="s">
+      <c r="A32" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="1" t="s">
+      <c r="A33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="1" t="s">
+      <c r="A34" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="s">
+      <c r="A35" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="37">
-      <c r="A37" s="1" t="s">
+      <c r="A37" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="38">
-      <c r="A38" s="1" t="s">
+      <c r="A38" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="39">
-      <c r="A39" s="1" t="s">
+      <c r="A39" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="40">
-      <c r="A40" s="1" t="s">
+      <c r="A40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="1" t="s">
+      <c r="A41" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="43">
-      <c r="A43" s="1" t="s">
+      <c r="A43" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B43" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="44">
-      <c r="A44" s="1" t="s">
+      <c r="A44" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B44" s="1" t="s">
+      <c r="B44" s="2" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="1" t="s">
+      <c r="A45" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="46">
-      <c r="A46" s="1" t="s">
+      <c r="A46" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="47">
-      <c r="A47" s="1" t="s">
+      <c r="A47" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="48">
-      <c r="A48" s="1" t="s">
+      <c r="A48" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="B48" s="1" t="s">
+      <c r="B48" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="49">
-      <c r="A49" s="1" t="s">
+      <c r="A49" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="50">
-      <c r="A50" s="1" t="s">
+      <c r="A50" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="1" t="s">
+      <c r="A51" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="s">
+      <c r="A52" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B52" s="1" t="s">
+      <c r="B52" s="2" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="53">
-      <c r="A53" s="1" t="s">
+      <c r="A53" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="B53" s="2" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" s="1" t="s">
+      <c r="A54" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="2" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="55">
-      <c r="A55" s="1" t="s">
+      <c r="A55" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="56">
-      <c r="A56" s="1" t="s">
+      <c r="A56" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="B56" s="1" t="s">
+      <c r="B56" s="2" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="57">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B57" s="1" t="s">
+      <c r="B57" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="58">
-      <c r="A58" s="1" t="s">
+      <c r="A58" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="1" t="s">
+      <c r="A59" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="60">
-      <c r="A60" s="1" t="s">
+      <c r="A60" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="B60" s="1" t="s">
+      <c r="B60" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="61">
-      <c r="A61" s="1" t="s">
+      <c r="A61" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="B61" s="1" t="s">
+      <c r="B61" s="2" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="62">
-      <c r="A62" s="1" t="s">
+      <c r="A62" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="1" t="s">
-        <v>121</v>
+      <c r="B62" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="63">
-      <c r="A63" s="1" t="s">
+      <c r="A63" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="1" t="s">
-        <v>124</v>
-      </c>
     </row>
     <row r="64">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="2" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="65">
-      <c r="A65" s="1" t="s">
+      <c r="A65" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B65" s="1" t="s">
+      <c r="B65" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="66">
-      <c r="A66" s="1" t="s">
+      <c r="A66" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="1" t="s">
+      <c r="B66" s="2" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="67">
-      <c r="A67" s="1" t="s">
+      <c r="A67" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="B67" s="1" t="s">
+      <c r="B67" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="68">
-      <c r="A68" s="1" t="s">
+      <c r="A68" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="2" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="69">
-      <c r="A69" s="1" t="s">
+      <c r="A69" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="B69" s="1" t="s">
+      <c r="B69" s="2" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="70">
-      <c r="A70" s="1" t="s">
+      <c r="A70" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B70" s="1" t="s">
+      <c r="B70" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="71">
-      <c r="A71" s="1" t="s">
+      <c r="A71" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="B71" s="1" t="s">
+      <c r="B71" s="2" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="72">
-      <c r="A72" s="1" t="s">
+      <c r="A72" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B72" s="1" t="s">
+      <c r="B72" s="2" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="73">
-      <c r="A73" s="1" t="s">
+      <c r="A73" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="2" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="74">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="B74" s="1" t="s">
+      <c r="B74" s="2" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="75">
-      <c r="A75" s="1" t="s">
+      <c r="A75" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="B75" s="1" t="s">
+      <c r="B75" s="2" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="76">
-      <c r="A76" s="1" t="s">
+      <c r="A76" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B76" s="1" t="s">
+      <c r="B76" s="2" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="77">
-      <c r="A77" s="1" t="s">
+      <c r="A77" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="78">
-      <c r="A78" s="1" t="s">
+      <c r="A78" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="1" t="s">
+      <c r="B78" s="2" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="79">
-      <c r="A79" s="1" t="s">
+      <c r="A79" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B79" s="1" t="s">
+      <c r="B79" s="2" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="80">
-      <c r="A80" s="1" t="s">
+      <c r="A80" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="2" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="B81" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>